<commit_message>
Actualizado v.7 y nuevos cambios de nombre, colores en gráficas y proyecto modular
</commit_message>
<xml_diff>
--- a/predictions/Valencia_Future_Predictions.xlsx
+++ b/predictions/Valencia_Future_Predictions.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -830,6 +830,123 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>08/01/2025</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>10.36499999999999</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>3.787</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>14.10400000000001</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.3799999999999998</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>265.15</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>12.206</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>27.40662903225803</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1015.845</v>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>09/01/2025</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>9.668999999999997</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>6.206</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>17.046</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.7440000000000001</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>289.39</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>15.147</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>27.81462903225803</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>1018.409</v>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>10/01/2025</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>12.037</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>3.449999999999999</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>13.979</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>1.573</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>278.96</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>16.84399999999999</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>27.34816129032254</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>1016.631</v>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>